<commit_message>
update readme file and script
</commit_message>
<xml_diff>
--- a/youtube_data.xlsx
+++ b/youtube_data.xlsx
@@ -1821,7 +1821,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>20187</t>
+          <t>20188</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1915,7 +1915,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>5416</t>
+          <t>5417</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>15881</t>
+          <t>15880</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -2616,7 +2616,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>67744</t>
+          <t>67743</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>19995</t>
+          <t>19997</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -2851,7 +2851,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>11906</t>
+          <t>11907</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">

</xml_diff>

<commit_message>
add pics in readme and remove id from comment replies
</commit_message>
<xml_diff>
--- a/youtube_data.xlsx
+++ b/youtube_data.xlsx
@@ -1821,7 +1821,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>20188</t>
+          <t>20191</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>7108</t>
+          <t>7109</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -2569,7 +2569,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>55141</t>
+          <t>55149</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -2616,7 +2616,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>67743</t>
+          <t>67753</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2710,7 +2710,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>1294675</t>
+          <t>1294683</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>19997</t>
+          <t>20001</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>26933</t>
+          <t>26949</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2851,7 +2851,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>11907</t>
+          <t>11908</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -3190,7 +3190,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>{'id': 'UgzqwArCEozFOJlbkOt4AaABAg', 'text': 'Thank you! Asphalt is trash, Concrete is the way to go. Flexible concrete is also very strong too. Where I live in Michigan, The concrete roads weren’t really done right and there are a bunch of potholes. On the concrete roads that they did right, it is actually still going strong. Also asphalt in Michigan doesn’t last for a long time. Maybe 10 to 15 years'}</t>
+          <t>Thank you! Asphalt is trash, Concrete is the way to go. Flexible concrete is also very strong too. Where I live in Michigan, The concrete roads weren’t really done right and there are a bunch of potholes. On the concrete roads that they did right, it is actually still going strong. Also asphalt in Michigan doesn’t last for a long time. Maybe 10 to 15 years</t>
         </is>
       </c>
     </row>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>{'id': 'UgzqwArCEozFOJlbkOt4AaABAg', 'text': 'Thank you! Asphalt is trash, Concrete is the way to go. Flexible concrete is also very strong too. Where I live in Michigan, The concrete roads weren’t really done right and there are a bunch of potholes. On the concrete roads that they did right, it is actually still going strong. Also asphalt in Michigan doesn’t last for a long time. Maybe 10 to 15 years'}</t>
+          <t>Thank you! Asphalt is trash, Concrete is the way to go. Flexible concrete is also very strong too. Where I live in Michigan, The concrete roads weren’t really done right and there are a bunch of potholes. On the concrete roads that they did right, it is actually still going strong. Also asphalt in Michigan doesn’t last for a long time. Maybe 10 to 15 years</t>
         </is>
       </c>
     </row>
@@ -3260,7 +3260,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>{'id': 'UgzqwArCEozFOJlbkOt4AaABAg', 'text': 'Thank you! Asphalt is trash, Concrete is the way to go. Flexible concrete is also very strong too. Where I live in Michigan, The concrete roads weren’t really done right and there are a bunch of potholes. On the concrete roads that they did right, it is actually still going strong. Also asphalt in Michigan doesn’t last for a long time. Maybe 10 to 15 years'}</t>
+          <t>Thank you! Asphalt is trash, Concrete is the way to go. Flexible concrete is also very strong too. Where I live in Michigan, The concrete roads weren’t really done right and there are a bunch of potholes. On the concrete roads that they did right, it is actually still going strong. Also asphalt in Michigan doesn’t last for a long time. Maybe 10 to 15 years</t>
         </is>
       </c>
     </row>
@@ -3295,7 +3295,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>{'id': 'UgzqwArCEozFOJlbkOt4AaABAg', 'text': 'Thank you! Asphalt is trash, Concrete is the way to go. Flexible concrete is also very strong too. Where I live in Michigan, The concrete roads weren’t really done right and there are a bunch of potholes. On the concrete roads that they did right, it is actually still going strong. Also asphalt in Michigan doesn’t last for a long time. Maybe 10 to 15 years'}</t>
+          <t>Thank you! Asphalt is trash, Concrete is the way to go. Flexible concrete is also very strong too. Where I live in Michigan, The concrete roads weren’t really done right and there are a bunch of potholes. On the concrete roads that they did right, it is actually still going strong. Also asphalt in Michigan doesn’t last for a long time. Maybe 10 to 15 years</t>
         </is>
       </c>
     </row>
@@ -3392,7 +3392,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>{'id': 'Ughr0AQ7HwbhCXgCoAEC', 'text': 'Asphalt might be okay in warm climate areas where there&amp;#39;s no snow salt or brine to damage it.'}</t>
+          <t>Asphalt might be okay in warm climate areas where there&amp;#39;s no snow salt or brine to damage it.</t>
         </is>
       </c>
     </row>
@@ -3458,7 +3458,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>{'id': 'UgiiEDZgTCYRungCoAEC', 'text': 'Brought to you by the unbiased lobby of Portland CEMENT association. :D'}</t>
+          <t>Brought to you by the unbiased lobby of Portland CEMENT association. :D</t>
         </is>
       </c>
     </row>
@@ -3493,7 +3493,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>{'id': 'UgiiEDZgTCYRungCoAEC', 'text': 'Brought to you by the unbiased lobby of Portland CEMENT association. :D'}</t>
+          <t>Brought to you by the unbiased lobby of Portland CEMENT association. :D</t>
         </is>
       </c>
     </row>
@@ -4181,7 +4181,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>{'id': 'Ugwu4IuJkoTc703CzrJ4AaABAg', 'text': 'This is being done near our location and I&amp;#39;m seeing an alarming amount of soil/dirt in the base mix. This does not sit well with my experience, but then again, I&amp;#39;m not an engineer.  Making concrete with top soil or dirt would not be my first choice of ingredient. Gravel and sand with cement would hold up better, as the contractor hauled in no additional base material for the road widening, they even just chewed up the side ditch dirt as the project calls for widening the road too. Not impressed with Milestone Contractors in Indiana.'}</t>
+          <t>This is being done near our location and I&amp;#39;m seeing an alarming amount of soil/dirt in the base mix. This does not sit well with my experience, but then again, I&amp;#39;m not an engineer.  Making concrete with top soil or dirt would not be my first choice of ingredient. Gravel and sand with cement would hold up better, as the contractor hauled in no additional base material for the road widening, they even just chewed up the side ditch dirt as the project calls for widening the road too. Not impressed with Milestone Contractors in Indiana.</t>
         </is>
       </c>
     </row>
@@ -4216,7 +4216,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>{'id': 'Ugwu4IuJkoTc703CzrJ4AaABAg', 'text': 'This is being done near our location and I&amp;#39;m seeing an alarming amount of soil/dirt in the base mix. This does not sit well with my experience, but then again, I&amp;#39;m not an engineer.  Making concrete with top soil or dirt would not be my first choice of ingredient. Gravel and sand with cement would hold up better, as the contractor hauled in no additional base material for the road widening, they even just chewed up the side ditch dirt as the project calls for widening the road too. Not impressed with Milestone Contractors in Indiana.'}</t>
+          <t>This is being done near our location and I&amp;#39;m seeing an alarming amount of soil/dirt in the base mix. This does not sit well with my experience, but then again, I&amp;#39;m not an engineer.  Making concrete with top soil or dirt would not be my first choice of ingredient. Gravel and sand with cement would hold up better, as the contractor hauled in no additional base material for the road widening, they even just chewed up the side ditch dirt as the project calls for widening the road too. Not impressed with Milestone Contractors in Indiana.</t>
         </is>
       </c>
     </row>
@@ -4251,7 +4251,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>{'id': 'Ugwu4IuJkoTc703CzrJ4AaABAg', 'text': 'This is being done near our location and I&amp;#39;m seeing an alarming amount of soil/dirt in the base mix. This does not sit well with my experience, but then again, I&amp;#39;m not an engineer.  Making concrete with top soil or dirt would not be my first choice of ingredient. Gravel and sand with cement would hold up better, as the contractor hauled in no additional base material for the road widening, they even just chewed up the side ditch dirt as the project calls for widening the road too. Not impressed with Milestone Contractors in Indiana.'}</t>
+          <t>This is being done near our location and I&amp;#39;m seeing an alarming amount of soil/dirt in the base mix. This does not sit well with my experience, but then again, I&amp;#39;m not an engineer.  Making concrete with top soil or dirt would not be my first choice of ingredient. Gravel and sand with cement would hold up better, as the contractor hauled in no additional base material for the road widening, they even just chewed up the side ditch dirt as the project calls for widening the road too. Not impressed with Milestone Contractors in Indiana.</t>
         </is>
       </c>
     </row>
@@ -4286,7 +4286,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>{'id': 'Ugwu4IuJkoTc703CzrJ4AaABAg', 'text': 'This is being done near our location and I&amp;#39;m seeing an alarming amount of soil/dirt in the base mix. This does not sit well with my experience, but then again, I&amp;#39;m not an engineer.  Making concrete with top soil or dirt would not be my first choice of ingredient. Gravel and sand with cement would hold up better, as the contractor hauled in no additional base material for the road widening, they even just chewed up the side ditch dirt as the project calls for widening the road too. Not impressed with Milestone Contractors in Indiana.'}</t>
+          <t>This is being done near our location and I&amp;#39;m seeing an alarming amount of soil/dirt in the base mix. This does not sit well with my experience, but then again, I&amp;#39;m not an engineer.  Making concrete with top soil or dirt would not be my first choice of ingredient. Gravel and sand with cement would hold up better, as the contractor hauled in no additional base material for the road widening, they even just chewed up the side ditch dirt as the project calls for widening the road too. Not impressed with Milestone Contractors in Indiana.</t>
         </is>
       </c>
     </row>
@@ -4321,7 +4321,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>{'id': 'Ugwu4IuJkoTc703CzrJ4AaABAg', 'text': 'This is being done near our location and I&amp;#39;m seeing an alarming amount of soil/dirt in the base mix. This does not sit well with my experience, but then again, I&amp;#39;m not an engineer.  Making concrete with top soil or dirt would not be my first choice of ingredient. Gravel and sand with cement would hold up better, as the contractor hauled in no additional base material for the road widening, they even just chewed up the side ditch dirt as the project calls for widening the road too. Not impressed with Milestone Contractors in Indiana.'}</t>
+          <t>This is being done near our location and I&amp;#39;m seeing an alarming amount of soil/dirt in the base mix. This does not sit well with my experience, but then again, I&amp;#39;m not an engineer.  Making concrete with top soil or dirt would not be my first choice of ingredient. Gravel and sand with cement would hold up better, as the contractor hauled in no additional base material for the road widening, they even just chewed up the side ditch dirt as the project calls for widening the road too. Not impressed with Milestone Contractors in Indiana.</t>
         </is>
       </c>
     </row>
@@ -4387,7 +4387,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>{'id': 'UgjAfTw2jvwDSXgCoAEC', 'text': 'If the existing road is bad because of a bad  base how will the new road be stronger?Your top is only as good as your bottom.'}</t>
+          <t>If the existing road is bad because of a bad  base how will the new road be stronger?Your top is only as good as your bottom.</t>
         </is>
       </c>
     </row>
@@ -4515,7 +4515,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>{'id': 'UgyjbmB27jclWw34ahN4AaABAg', 'text': 'A very good introduction to the wonder and miracle of concrete. Without it our modern day privileges would not exist.'}</t>
+          <t>A very good introduction to the wonder and miracle of concrete. Without it our modern day privileges would not exist.</t>
         </is>
       </c>
     </row>
@@ -4550,7 +4550,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>{'id': 'UgyjbmB27jclWw34ahN4AaABAg', 'text': 'A very good introduction to the wonder and miracle of concrete. Without it our modern day privileges would not exist.'}</t>
+          <t>A very good introduction to the wonder and miracle of concrete. Without it our modern day privileges would not exist.</t>
         </is>
       </c>
     </row>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>{'id': 'UgyBjwBevELwaJ8_15B4AaABAg', 'text': 'i&amp;#39;ve had eye problems for about a month. just realized it was the damn cement i was filling cracks with in my garage. Doh. mixing it indoors is a bad idea without proper ventilation and no goggles. i thought the powder was heavy enough that it wasn&amp;#39;t floating up to my eyes.'}</t>
+          <t>i&amp;#39;ve had eye problems for about a month. just realized it was the damn cement i was filling cracks with in my garage. Doh. mixing it indoors is a bad idea without proper ventilation and no goggles. i thought the powder was heavy enough that it wasn&amp;#39;t floating up to my eyes.</t>
         </is>
       </c>
     </row>
@@ -4837,7 +4837,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>{'id': 'UgyHORWpe_ikULMTwg54AaABAg', 'text': 'If there&amp;#39;s one thing my genes has.. and that is i&amp;#39;m immune to cement chemicals... i can literally take a bath with that cement....'}</t>
+          <t>If there&amp;#39;s one thing my genes has.. and that is i&amp;#39;m immune to cement chemicals... i can literally take a bath with that cement....</t>
         </is>
       </c>
     </row>
@@ -5058,7 +5058,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>{'id': 'Ugyh_UxdSVp665T4Vft4AaABAg', 'text': 'You would be surprised how many people are not aware of this. And I quote, &amp;#39;We use cement in everything. It&amp;#39;s not a dangerous substance until it dries.&amp;#39;'}</t>
+          <t>You would be surprised how many people are not aware of this. And I quote, &amp;#39;We use cement in everything. It&amp;#39;s not a dangerous substance until it dries.&amp;#39;</t>
         </is>
       </c>
     </row>
@@ -5124,7 +5124,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>{'id': 'UgysDQJVXN5A0JQcRP94AaABAg', 'text': 'So I’m a concrete finisher and we work with live cement and I’m not sure what I have but my right hand feels swollen I can’t close it completely and the joints on my fingers hurt. Not sure if that’s from using the float for hours or from the cement.'}</t>
+          <t>So I’m a concrete finisher and we work with live cement and I’m not sure what I have but my right hand feels swollen I can’t close it completely and the joints on my fingers hurt. Not sure if that’s from using the float for hours or from the cement.</t>
         </is>
       </c>
     </row>
@@ -5159,7 +5159,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>{'id': 'UgysDQJVXN5A0JQcRP94AaABAg', 'text': 'So I’m a concrete finisher and we work with live cement and I’m not sure what I have but my right hand feels swollen I can’t close it completely and the joints on my fingers hurt. Not sure if that’s from using the float for hours or from the cement.'}</t>
+          <t>So I’m a concrete finisher and we work with live cement and I’m not sure what I have but my right hand feels swollen I can’t close it completely and the joints on my fingers hurt. Not sure if that’s from using the float for hours or from the cement.</t>
         </is>
       </c>
     </row>
@@ -5256,7 +5256,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>{'id': 'UggZk2TUR0FyOngCoAEC', 'text': 'Hi - I&amp;#39;m Troy McClure, you may remember me from such educational films as: &amp;quot;The Half-Assed Approach to Foundation Repair&amp;quot; and &amp;quot;Lead Paint: Delicious But Deadly&amp;quot;'}</t>
+          <t>Hi - I&amp;#39;m Troy McClure, you may remember me from such educational films as: &amp;quot;The Half-Assed Approach to Foundation Repair&amp;quot; and &amp;quot;Lead Paint: Delicious But Deadly&amp;quot;</t>
         </is>
       </c>
     </row>
@@ -5291,7 +5291,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>{'id': 'UggZk2TUR0FyOngCoAEC', 'text': 'Hi - I&amp;#39;m Troy McClure, you may remember me from such educational films as: &amp;quot;The Half-Assed Approach to Foundation Repair&amp;quot; and &amp;quot;Lead Paint: Delicious But Deadly&amp;quot;'}</t>
+          <t>Hi - I&amp;#39;m Troy McClure, you may remember me from such educational films as: &amp;quot;The Half-Assed Approach to Foundation Repair&amp;quot; and &amp;quot;Lead Paint: Delicious But Deadly&amp;quot;</t>
         </is>
       </c>
     </row>
@@ -5388,7 +5388,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>{'id': 'Ugzz2j6ES7nVVALv6U14AaABAg', 'text': 'Kind Referee, check for soil report, look for loose debris, Rebar tags, wire, rocks and trash. Have the current Plans and any RFIs or changes made to the area to be inspected.  Look for simple presentation, is there proper clearance? Is the size of the bar and spacing correct?  Is the lap splice correct? Lap splice will change if the PSI of the concrete is 3k or 5k? Check lap schedule. Read general notes!! And if you are on my job give me a break!!'}</t>
+          <t>Kind Referee, check for soil report, look for loose debris, Rebar tags, wire, rocks and trash. Have the current Plans and any RFIs or changes made to the area to be inspected.  Look for simple presentation, is there proper clearance? Is the size of the bar and spacing correct?  Is the lap splice correct? Lap splice will change if the PSI of the concrete is 3k or 5k? Check lap schedule. Read general notes!! And if you are on my job give me a break!!</t>
         </is>
       </c>
     </row>
@@ -5454,7 +5454,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>{'id': 'UgwlPZATXhCY8KKPqXJ4AaABAg', 'text': 'What is the remedy if there are rust on the installed reinforcement?'}</t>
+          <t>What is the remedy if there are rust on the installed reinforcement?</t>
         </is>
       </c>
     </row>
@@ -5489,7 +5489,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>{'id': 'UgwlPZATXhCY8KKPqXJ4AaABAg', 'text': 'What is the remedy if there are rust on the installed reinforcement?'}</t>
+          <t>What is the remedy if there are rust on the installed reinforcement?</t>
         </is>
       </c>
     </row>
@@ -5617,7 +5617,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>{'id': 'UgwhCO3HLjtI5VeQN8h4AaABAg', 'text': 'If tie-wire has oil?&lt;br&gt; What should we do??'}</t>
+          <t>If tie-wire has oil?&lt;br&gt; What should we do??</t>
         </is>
       </c>
     </row>
@@ -5776,7 +5776,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>{'id': 'Ugz78AXt8hvn1_TZP4R4AaABAg', 'text': 'i&amp;#39;m watching because tomorrow is my first day as an inspector. Oh boy Im nervous lool'}</t>
+          <t>i&amp;#39;m watching because tomorrow is my first day as an inspector. Oh boy Im nervous lool</t>
         </is>
       </c>
     </row>
@@ -5811,7 +5811,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>{'id': 'Ugz78AXt8hvn1_TZP4R4AaABAg', 'text': 'i&amp;#39;m watching because tomorrow is my first day as an inspector. Oh boy Im nervous lool'}</t>
+          <t>i&amp;#39;m watching because tomorrow is my first day as an inspector. Oh boy Im nervous lool</t>
         </is>
       </c>
     </row>
@@ -6187,7 +6187,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>{'id': 'UgwkK_zsEXEKpEz4hLp4AaABAg', 'text': 'One thing that has always intrigued me is why plastic ties are not used to connect reinforcing together prior to pouring the concrete.  Extensive enquiries here in New Zealand have always drawn the same response:  it is not known what the structural importance of steel tie wire is,  and it is not known what the objection to plastic ties might be.  Can you throw any light on this issue?  Regards from NZ'}</t>
+          <t>One thing that has always intrigued me is why plastic ties are not used to connect reinforcing together prior to pouring the concrete.  Extensive enquiries here in New Zealand have always drawn the same response:  it is not known what the structural importance of steel tie wire is,  and it is not known what the objection to plastic ties might be.  Can you throw any light on this issue?  Regards from NZ</t>
         </is>
       </c>
     </row>
@@ -6222,7 +6222,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>{'id': 'UgwkK_zsEXEKpEz4hLp4AaABAg', 'text': 'One thing that has always intrigued me is why plastic ties are not used to connect reinforcing together prior to pouring the concrete.  Extensive enquiries here in New Zealand have always drawn the same response:  it is not known what the structural importance of steel tie wire is,  and it is not known what the objection to plastic ties might be.  Can you throw any light on this issue?  Regards from NZ'}</t>
+          <t>One thing that has always intrigued me is why plastic ties are not used to connect reinforcing together prior to pouring the concrete.  Extensive enquiries here in New Zealand have always drawn the same response:  it is not known what the structural importance of steel tie wire is,  and it is not known what the objection to plastic ties might be.  Can you throw any light on this issue?  Regards from NZ</t>
         </is>
       </c>
     </row>
@@ -6257,7 +6257,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>{'id': 'UgwkK_zsEXEKpEz4hLp4AaABAg', 'text': 'One thing that has always intrigued me is why plastic ties are not used to connect reinforcing together prior to pouring the concrete.  Extensive enquiries here in New Zealand have always drawn the same response:  it is not known what the structural importance of steel tie wire is,  and it is not known what the objection to plastic ties might be.  Can you throw any light on this issue?  Regards from NZ'}</t>
+          <t>One thing that has always intrigued me is why plastic ties are not used to connect reinforcing together prior to pouring the concrete.  Extensive enquiries here in New Zealand have always drawn the same response:  it is not known what the structural importance of steel tie wire is,  and it is not known what the objection to plastic ties might be.  Can you throw any light on this issue?  Regards from NZ</t>
         </is>
       </c>
     </row>
@@ -6292,7 +6292,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>{'id': 'UgwkK_zsEXEKpEz4hLp4AaABAg', 'text': 'One thing that has always intrigued me is why plastic ties are not used to connect reinforcing together prior to pouring the concrete.  Extensive enquiries here in New Zealand have always drawn the same response:  it is not known what the structural importance of steel tie wire is,  and it is not known what the objection to plastic ties might be.  Can you throw any light on this issue?  Regards from NZ'}</t>
+          <t>One thing that has always intrigued me is why plastic ties are not used to connect reinforcing together prior to pouring the concrete.  Extensive enquiries here in New Zealand have always drawn the same response:  it is not known what the structural importance of steel tie wire is,  and it is not known what the objection to plastic ties might be.  Can you throw any light on this issue?  Regards from NZ</t>
         </is>
       </c>
     </row>
@@ -6637,7 +6637,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>{'id': 'Ugz5RHGovY-EJ8a9Yzd4AaABAg', 'text': 'Thank you very much, now I am more afraid to do anything with concrete at all. If even adding a little bit of water is such a problem. You overcomplicated it for me. Around me are many guys who built houses without knowing too much.'}</t>
+          <t>Thank you very much, now I am more afraid to do anything with concrete at all. If even adding a little bit of water is such a problem. You overcomplicated it for me. Around me are many guys who built houses without knowing too much.</t>
         </is>
       </c>
     </row>
@@ -7478,7 +7478,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>{'id': 'Ugyuoeg46eCYW1pVzvd4AaABAg', 'text': 'When pouring concrete do you take into consideration the curvature f the eaarh the math is 8inch per mile squared. 666 feet per 10 miles. I had never learned of this curvature. I&amp;#39;ve always built stuff on  a level plain.'}</t>
+          <t>When pouring concrete do you take into consideration the curvature f the eaarh the math is 8inch per mile squared. 666 feet per 10 miles. I had never learned of this curvature. I&amp;#39;ve always built stuff on  a level plain.</t>
         </is>
       </c>
     </row>
@@ -7513,7 +7513,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>{'id': 'Ugyuoeg46eCYW1pVzvd4AaABAg', 'text': 'When pouring concrete do you take into consideration the curvature f the eaarh the math is 8inch per mile squared. 666 feet per 10 miles. I had never learned of this curvature. I&amp;#39;ve always built stuff on  a level plain.'}</t>
+          <t>When pouring concrete do you take into consideration the curvature f the eaarh the math is 8inch per mile squared. 666 feet per 10 miles. I had never learned of this curvature. I&amp;#39;ve always built stuff on  a level plain.</t>
         </is>
       </c>
     </row>
@@ -7610,7 +7610,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>{'id': 'UgyfgHJWgSwKvg2QekJ4AaABAg', 'text': 'If i ever saw a finisher walk on a placement to determine when to finish, that would the last job of mine he ever worked on!'}</t>
+          <t>If i ever saw a finisher walk on a placement to determine when to finish, that would the last job of mine he ever worked on!</t>
         </is>
       </c>
     </row>
@@ -7645,7 +7645,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>{'id': 'UgyfgHJWgSwKvg2QekJ4AaABAg', 'text': 'If i ever saw a finisher walk on a placement to determine when to finish, that would the last job of mine he ever worked on!'}</t>
+          <t>If i ever saw a finisher walk on a placement to determine when to finish, that would the last job of mine he ever worked on!</t>
         </is>
       </c>
     </row>
@@ -7680,7 +7680,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>{'id': 'UgyfgHJWgSwKvg2QekJ4AaABAg', 'text': 'If i ever saw a finisher walk on a placement to determine when to finish, that would the last job of mine he ever worked on!'}</t>
+          <t>If i ever saw a finisher walk on a placement to determine when to finish, that would the last job of mine he ever worked on!</t>
         </is>
       </c>
     </row>
@@ -7715,7 +7715,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>{'id': 'UgyfgHJWgSwKvg2QekJ4AaABAg', 'text': 'If i ever saw a finisher walk on a placement to determine when to finish, that would the last job of mine he ever worked on!'}</t>
+          <t>If i ever saw a finisher walk on a placement to determine when to finish, that would the last job of mine he ever worked on!</t>
         </is>
       </c>
     </row>
@@ -7781,7 +7781,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>{'id': 'Ugwc-FtQz9ep9EgJt6l4AaABAg', 'text': 'I would specify like this, give me 4000 psi @ 4 1/2&amp;quot; slump with air between 3 and 6%'}</t>
+          <t>I would specify like this, give me 4000 psi @ 4 1/2&amp;quot; slump with air between 3 and 6%</t>
         </is>
       </c>
     </row>
@@ -7847,7 +7847,7 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>{'id': 'Ugyc6yHHgpeTHA0f0PV4AaABAg', 'text': 'You know I was in the building trades for many years.....and many of my years was building houses in Ohio...in cold weather......we had to deal with the Masons......all the time.............building on the concrete slabs........lol......./oh yeah can’t do that because of this or this or. Ya put this wall up till the wall till the concrete is firm go home ect.........lol....all the time...they would get behind because of the weather....and they just can’t pour because of the weather ect......or they couldn’t get. A truck into the site of mud.......so the foundation would be just be setting up....so we would be behind.......it was ready for concrete.....but no truck??'}</t>
+          <t>You know I was in the building trades for many years.....and many of my years was building houses in Ohio...in cold weather......we had to deal with the Masons......all the time.............building on the concrete slabs........lol......./oh yeah can’t do that because of this or this or. Ya put this wall up till the wall till the concrete is firm go home ect.........lol....all the time...they would get behind because of the weather....and they just can’t pour because of the weather ect......or they couldn’t get. A truck into the site of mud.......so the foundation would be just be setting up....so we would be behind.......it was ready for concrete.....but no truck??</t>
         </is>
       </c>
     </row>
@@ -7944,7 +7944,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>{'id': 'UgyX5VbYTakKVW9nfkV4AaABAg', 'text': 'No. 1 of the Top Ten Myths of Concrete -  “ All concrete cracks”'}</t>
+          <t>No. 1 of the Top Ten Myths of Concrete -  “ All concrete cracks”</t>
         </is>
       </c>
     </row>
@@ -7979,7 +7979,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>{'id': 'UgyX5VbYTakKVW9nfkV4AaABAg', 'text': 'No. 1 of the Top Ten Myths of Concrete -  “ All concrete cracks”'}</t>
+          <t>No. 1 of the Top Ten Myths of Concrete -  “ All concrete cracks”</t>
         </is>
       </c>
     </row>
@@ -8014,7 +8014,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>{'id': 'UgyX5VbYTakKVW9nfkV4AaABAg', 'text': 'No. 1 of the Top Ten Myths of Concrete -  “ All concrete cracks”'}</t>
+          <t>No. 1 of the Top Ten Myths of Concrete -  “ All concrete cracks”</t>
         </is>
       </c>
     </row>
@@ -8049,7 +8049,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>{'id': 'UgyX5VbYTakKVW9nfkV4AaABAg', 'text': 'No. 1 of the Top Ten Myths of Concrete -  “ All concrete cracks”'}</t>
+          <t>No. 1 of the Top Ten Myths of Concrete -  “ All concrete cracks”</t>
         </is>
       </c>
     </row>
@@ -8084,7 +8084,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>{'id': 'UgyX5VbYTakKVW9nfkV4AaABAg', 'text': 'No. 1 of the Top Ten Myths of Concrete -  “ All concrete cracks”'}</t>
+          <t>No. 1 of the Top Ten Myths of Concrete -  “ All concrete cracks”</t>
         </is>
       </c>
     </row>
@@ -8646,7 +8646,7 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>{'id': 'Ugye0V0PHiwJJuYy-Tp4AaABAg', 'text': 'Amazing how the old world [ romans] could make concrete that has lasted a 1000 years and is still strong . But now the concrete companies can&amp;#39;t get their stuff past a service lifetime of 50 years before it starts cracking and cumbling  . It must be called profits .'}</t>
+          <t>Amazing how the old world [ romans] could make concrete that has lasted a 1000 years and is still strong . But now the concrete companies can&amp;#39;t get their stuff past a service lifetime of 50 years before it starts cracking and cumbling  . It must be called profits .</t>
         </is>
       </c>
     </row>
@@ -8681,7 +8681,7 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>{'id': 'Ugye0V0PHiwJJuYy-Tp4AaABAg', 'text': 'Amazing how the old world [ romans] could make concrete that has lasted a 1000 years and is still strong . But now the concrete companies can&amp;#39;t get their stuff past a service lifetime of 50 years before it starts cracking and cumbling  . It must be called profits .'}</t>
+          <t>Amazing how the old world [ romans] could make concrete that has lasted a 1000 years and is still strong . But now the concrete companies can&amp;#39;t get their stuff past a service lifetime of 50 years before it starts cracking and cumbling  . It must be called profits .</t>
         </is>
       </c>
     </row>
@@ -8933,7 +8933,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>{'id': 'Ugx1RjYI2W4xLF1FUzx4AaABAg', 'text': 'The mash Des&amp;quot;t'}</t>
+          <t>The mash Des&amp;quot;t</t>
         </is>
       </c>
     </row>
@@ -9030,7 +9030,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>{'id': 'UgxaLtYx6brjhzz8KOB4AaABAg', 'text': 'The last good pour, with perfect slump, was back in Greece 500BC. Today science is getting close to recreating that batch in the lab.'}</t>
+          <t>The last good pour, with perfect slump, was back in Greece 500BC. Today science is getting close to recreating that batch in the lab.</t>
         </is>
       </c>
     </row>
@@ -9065,7 +9065,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>{'id': 'UgxaLtYx6brjhzz8KOB4AaABAg', 'text': 'The last good pour, with perfect slump, was back in Greece 500BC. Today science is getting close to recreating that batch in the lab.'}</t>
+          <t>The last good pour, with perfect slump, was back in Greece 500BC. Today science is getting close to recreating that batch in the lab.</t>
         </is>
       </c>
     </row>
@@ -9255,7 +9255,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>{'id': 'Ugxgm0qamUvq3ShAdnB4AaABAg', 'text': 'why do you put the rebar mash on the ground and then put the concrete over it?'}</t>
+          <t>why do you put the rebar mash on the ground and then put the concrete over it?</t>
         </is>
       </c>
     </row>
@@ -9538,7 +9538,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>{'id': 'UgxFx9KcmPsusA-WlJ94AaABAg', 'text': 'This video confirms my opinion that laying concrete is not for amateurs. The only thing I will do is put in a fence post.'}</t>
+          <t>This video confirms my opinion that laying concrete is not for amateurs. The only thing I will do is put in a fence post.</t>
         </is>
       </c>
     </row>
@@ -9666,7 +9666,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>{'id': 'UgyGNmv1itxr7YMU9zB4AaABAg', 'text': 'Being a cement finisher brought me here.'}</t>
+          <t>Being a cement finisher brought me here.</t>
         </is>
       </c>
     </row>
@@ -10104,7 +10104,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>{'id': 'UgzzJ5a44_AvhlpnGCt4AaABAg', 'text': 'My only gripe is the &amp;quot;Cement Mill&amp;quot; shown is a cement kiln!'}</t>
+          <t>My only gripe is the &amp;quot;Cement Mill&amp;quot; shown is a cement kiln!</t>
         </is>
       </c>
     </row>
@@ -10201,7 +10201,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>{'id': 'Ugjz46QOJUUztHgCoAEC', 'text': 'Is distilled water used in Concrete some time ?'}</t>
+          <t>Is distilled water used in Concrete some time ?</t>
         </is>
       </c>
     </row>
@@ -10391,7 +10391,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>{'id': 'UgztTDasqaTMDOB1xqR4AaABAg', 'text': 'What type of filler would you use it looked like some gravel? Is there a primer you would use prior to the concrete overlay?'}</t>
+          <t>What type of filler would you use it looked like some gravel? Is there a primer you would use prior to the concrete overlay?</t>
         </is>
       </c>
     </row>

</xml_diff>